<commit_message>
added in 3 new SRA numbers fro drosRTEC data
</commit_message>
<xml_diff>
--- a/populationInfo/vcf_popinfo_Oct2018.xlsx
+++ b/populationInfo/vcf_popinfo_Oct2018.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanbergland/Documents/GitHub/DEST/populationInfo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73222D29-5F14-E446-93BA-97F5D3CD9D0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B005304F-2626-D549-8512-DA3AE3DB266D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10540" yWindow="460" windowWidth="35640" windowHeight="19180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13460" yWindow="460" windowWidth="35640" windowHeight="19180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="popinfo.txt" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="438">
   <si>
     <t>mel159_112012_CO</t>
   </si>
@@ -1343,13 +1343,22 @@
   </si>
   <si>
     <t>D. Promislow</t>
+  </si>
+  <si>
+    <t>SRX8295554</t>
+  </si>
+  <si>
+    <t>SRX8295556</t>
+  </si>
+  <si>
+    <t>SRX8295555</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1408,6 +1417,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1653,7 +1668,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1664,6 +1679,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="219">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2224,10 +2240,10 @@
   <dimension ref="A1:AA78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="L70" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="AA42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L78" sqref="L78"/>
+      <selection pane="bottomRight" activeCell="AA78" sqref="AA78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2235,13 +2251,13 @@
     <col min="1" max="1" width="19.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="25.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" style="2" customWidth="1"/>
-    <col min="7" max="18" width="10.83203125" style="1"/>
-    <col min="19" max="19" width="17" style="1" customWidth="1"/>
-    <col min="20" max="20" width="24.6640625" style="1" customWidth="1"/>
-    <col min="21" max="24" width="10.83203125" style="1"/>
-    <col min="25" max="26" width="10" style="1" customWidth="1"/>
+    <col min="4" max="5" width="25.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="18" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="17" style="1" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="24.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="21" max="24" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="25" max="26" width="10" style="1" hidden="1" customWidth="1"/>
     <col min="27" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -2490,6 +2506,9 @@
       <c r="Z3" s="1">
         <v>40.4</v>
       </c>
+      <c r="AA3" s="10" t="s">
+        <v>435</v>
+      </c>
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -8629,11 +8648,11 @@
       <c r="Z77" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AA77" s="1" t="s">
-        <v>72</v>
+      <c r="AA77" s="10" t="s">
+        <v>436</v>
       </c>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>427</v>
       </c>
@@ -8712,8 +8731,8 @@
       <c r="Z78" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AA78" s="1" t="s">
-        <v>72</v>
+      <c r="AA78" s="10" t="s">
+        <v>437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
drosRTEC sample name updates
</commit_message>
<xml_diff>
--- a/populationInfo/vcf_popinfo_Oct2018.xlsx
+++ b/populationInfo/vcf_popinfo_Oct2018.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanbergland/Documents/GitHub/DEST/populationInfo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA2DE35-0CCC-8041-8553-D220D2D23C2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950BB950-010F-A144-88CE-2A853F3BDDFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16620" yWindow="460" windowWidth="35640" windowHeight="19180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12860" yWindow="460" windowWidth="35640" windowHeight="19180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="popinfo.txt" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="461">
   <si>
     <t>mel159_112012_CO</t>
   </si>
@@ -1415,6 +1415,12 @@
   </si>
   <si>
     <t>PA_7_2011</t>
+  </si>
+  <si>
+    <t>PA_10_2012</t>
+  </si>
+  <si>
+    <t>mel14TWA7</t>
   </si>
 </sst>
 </file>
@@ -2303,10 +2309,10 @@
   <dimension ref="A1:AB78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2508,7 +2514,7 @@
         <v>314</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>390</v>
+        <v>460</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>390</v>
@@ -8954,8 +8960,8 @@
       <c r="C78" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D78" s="7" t="s">
-        <v>412</v>
+      <c r="D78" t="s">
+        <v>459</v>
       </c>
       <c r="E78" s="7" t="s">
         <v>412</v>

</xml_diff>